<commit_message>
[Hall Effect] Add figs calibration, update jupyter notebook and fix combined datasets
</commit_message>
<xml_diff>
--- a/Hall/Combined_dataset.xlsx
+++ b/Hall/Combined_dataset.xlsx
@@ -399,10 +399,10 @@
         <v>11.8</v>
       </c>
       <c r="D2" t="n">
-        <v>-1520</v>
+        <v>1520</v>
       </c>
       <c r="E2" t="n">
-        <v>-2230</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="3">
@@ -416,10 +416,10 @@
         <v>10.3</v>
       </c>
       <c r="D3" t="n">
-        <v>-1290</v>
+        <v>1290</v>
       </c>
       <c r="E3" t="n">
-        <v>-1940</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="4">
@@ -433,10 +433,10 @@
         <v>8.400000000000006</v>
       </c>
       <c r="D4" t="n">
-        <v>-1056</v>
+        <v>1056</v>
       </c>
       <c r="E4" t="n">
-        <v>-1560</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="5">
@@ -450,10 +450,10 @@
         <v>7.100000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>-895.1</v>
+        <v>895.1</v>
       </c>
       <c r="E5" t="n">
-        <v>-1350</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="6">
@@ -467,10 +467,10 @@
         <v>6.100000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>-777.5</v>
+        <v>777.5</v>
       </c>
       <c r="E6" t="n">
-        <v>-1171</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="7">
@@ -484,10 +484,10 @@
         <v>5.48</v>
       </c>
       <c r="D7" t="n">
-        <v>-688.7</v>
+        <v>688.7</v>
       </c>
       <c r="E7" t="n">
-        <v>-1034.5</v>
+        <v>1034.5</v>
       </c>
     </row>
     <row r="8">
@@ -501,10 +501,10 @@
         <v>4.830000000000002</v>
       </c>
       <c r="D8" t="n">
-        <v>-618.9</v>
+        <v>618.9</v>
       </c>
       <c r="E8" t="n">
-        <v>-927.5</v>
+        <v>927.5</v>
       </c>
     </row>
     <row r="9">
@@ -518,10 +518,10 @@
         <v>4.34</v>
       </c>
       <c r="D9" t="n">
-        <v>-563.3</v>
+        <v>563.3</v>
       </c>
       <c r="E9" t="n">
-        <v>-841.5</v>
+        <v>841.5</v>
       </c>
     </row>
     <row r="10">
@@ -535,10 +535,10 @@
         <v>3.91</v>
       </c>
       <c r="D10" t="n">
-        <v>-518.3</v>
+        <v>518.3</v>
       </c>
       <c r="E10" t="n">
-        <v>-771.3</v>
+        <v>771.3</v>
       </c>
     </row>
     <row r="11">
@@ -552,10 +552,10 @@
         <v>3.619999999999997</v>
       </c>
       <c r="D11" t="n">
-        <v>-481.1999999999999</v>
+        <v>481.1999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>-713.3</v>
+        <v>713.3</v>
       </c>
     </row>
     <row r="12">
@@ -569,10 +569,10 @@
         <v>3.359999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>-450.9</v>
+        <v>450.9</v>
       </c>
       <c r="E12" t="n">
-        <v>-665.6999999999999</v>
+        <v>665.6999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -586,10 +586,10 @@
         <v>3.120000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>-426</v>
+        <v>426</v>
       </c>
       <c r="E13" t="n">
-        <v>-626.5999999999999</v>
+        <v>626.5999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -603,10 +603,10 @@
         <v>2.93</v>
       </c>
       <c r="D14" t="n">
-        <v>-404.7</v>
+        <v>404.7</v>
       </c>
       <c r="E14" t="n">
-        <v>-592.8</v>
+        <v>592.8</v>
       </c>
     </row>
     <row r="15">
@@ -620,10 +620,10 @@
         <v>2.729999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>-387.2</v>
+        <v>387.2</v>
       </c>
       <c r="E15" t="n">
-        <v>-564.9</v>
+        <v>564.9</v>
       </c>
     </row>
     <row r="16">
@@ -637,10 +637,10 @@
         <v>2.529999999999999</v>
       </c>
       <c r="D16" t="n">
-        <v>-372.1</v>
+        <v>372.1</v>
       </c>
       <c r="E16" t="n">
-        <v>-540.6999999999999</v>
+        <v>540.6999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -654,10 +654,10 @@
         <v>2.436999999999999</v>
       </c>
       <c r="D17" t="n">
-        <v>-359.92</v>
+        <v>359.92</v>
       </c>
       <c r="E17" t="n">
-        <v>-521.0799999999999</v>
+        <v>521.0799999999999</v>
       </c>
     </row>
     <row r="18">
@@ -671,10 +671,10 @@
         <v>2.322999999999999</v>
       </c>
       <c r="D18" t="n">
-        <v>-349.53</v>
+        <v>349.53</v>
       </c>
       <c r="E18" t="n">
-        <v>-503.95</v>
+        <v>503.95</v>
       </c>
     </row>
     <row r="19">
@@ -688,10 +688,10 @@
         <v>2.215</v>
       </c>
       <c r="D19" t="n">
-        <v>-340.85</v>
+        <v>340.85</v>
       </c>
       <c r="E19" t="n">
-        <v>-489.35</v>
+        <v>489.35</v>
       </c>
     </row>
     <row r="20">
@@ -705,10 +705,10 @@
         <v>2.091000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>-333.54</v>
+        <v>333.54</v>
       </c>
       <c r="E20" t="n">
-        <v>-477.19</v>
+        <v>477.19</v>
       </c>
     </row>
     <row r="21">
@@ -722,10 +722,10 @@
         <v>2.037999999999998</v>
       </c>
       <c r="D21" t="n">
-        <v>-327.2699999999999</v>
+        <v>327.2699999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>-466.3</v>
+        <v>466.3</v>
       </c>
     </row>
     <row r="22">
@@ -739,10 +739,10 @@
         <v>1.960000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>-322.67</v>
+        <v>322.67</v>
       </c>
       <c r="E22" t="n">
-        <v>-458.04</v>
+        <v>458.04</v>
       </c>
     </row>
     <row r="23">
@@ -756,10 +756,10 @@
         <v>1.889000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>-318.76</v>
+        <v>318.76</v>
       </c>
       <c r="E23" t="n">
-        <v>-450.73</v>
+        <v>450.73</v>
       </c>
     </row>
     <row r="24">
@@ -773,10 +773,10 @@
         <v>1.798</v>
       </c>
       <c r="D24" t="n">
-        <v>-315.4299999999999</v>
+        <v>315.4299999999999</v>
       </c>
       <c r="E24" t="n">
-        <v>-444.26</v>
+        <v>444.26</v>
       </c>
     </row>
     <row r="25">
@@ -790,10 +790,10 @@
         <v>1.729000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>-313.12</v>
+        <v>313.12</v>
       </c>
       <c r="E25" t="n">
-        <v>-439.27</v>
+        <v>439.27</v>
       </c>
     </row>
     <row r="26">
@@ -807,10 +807,10 @@
         <v>1.711</v>
       </c>
       <c r="D26" t="n">
-        <v>-311.4999999999999</v>
+        <v>311.4999999999999</v>
       </c>
       <c r="E26" t="n">
-        <v>-435.1899999999999</v>
+        <v>435.1899999999999</v>
       </c>
     </row>
     <row r="27">
@@ -821,13 +821,13 @@
         <v>203</v>
       </c>
       <c r="C27" t="n">
-        <v>1.600000381469727</v>
+        <v>1.6</v>
       </c>
       <c r="D27" t="n">
-        <v>-310</v>
+        <v>310</v>
       </c>
       <c r="E27" t="n">
-        <v>-430.9999694824219</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28">
@@ -841,10 +841,10 @@
         <v>1.5</v>
       </c>
       <c r="D28" t="n">
-        <v>-309</v>
+        <v>308.9999999999999</v>
       </c>
       <c r="E28" t="n">
-        <v>-429</v>
+        <v>428.9999999999999</v>
       </c>
     </row>
     <row r="29">
@@ -858,10 +858,10 @@
         <v>1.5</v>
       </c>
       <c r="D29" t="n">
-        <v>-310</v>
+        <v>310</v>
       </c>
       <c r="E29" t="n">
-        <v>-427</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30">
@@ -875,10 +875,10 @@
         <v>1.5</v>
       </c>
       <c r="D30" t="n">
-        <v>-311</v>
+        <v>311</v>
       </c>
       <c r="E30" t="n">
-        <v>-425.9999694824219</v>
+        <v>426</v>
       </c>
     </row>
     <row r="31">
@@ -889,13 +889,13 @@
         <v>223</v>
       </c>
       <c r="C31" t="n">
-        <v>1.380000114440918</v>
+        <v>1.379999999999999</v>
       </c>
       <c r="D31" t="n">
-        <v>-312</v>
+        <v>312</v>
       </c>
       <c r="E31" t="n">
-        <v>-425.9999694824219</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32">
@@ -906,13 +906,13 @@
         <v>228</v>
       </c>
       <c r="C32" t="n">
-        <v>1.40000057220459</v>
+        <v>1.4</v>
       </c>
       <c r="D32" t="n">
-        <v>-314</v>
+        <v>313.9999999999999</v>
       </c>
       <c r="E32" t="n">
-        <v>425.9999694824219</v>
+        <v>426</v>
       </c>
     </row>
     <row r="33">
@@ -923,13 +923,13 @@
         <v>233</v>
       </c>
       <c r="C33" t="n">
-        <v>1.399999618530273</v>
+        <v>1.4</v>
       </c>
       <c r="D33" t="n">
-        <v>-316</v>
+        <v>316</v>
       </c>
       <c r="E33" t="n">
-        <v>-425.9999694824219</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34">
@@ -940,13 +940,13 @@
         <v>238</v>
       </c>
       <c r="C34" t="n">
-        <v>1.300000190734863</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>-318</v>
+        <v>318</v>
       </c>
       <c r="E34" t="n">
-        <v>-427</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35">
@@ -957,13 +957,13 @@
         <v>244</v>
       </c>
       <c r="C35" t="n">
-        <v>1.300000190734863</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="D35" t="n">
-        <v>-320.9999694824219</v>
+        <v>321</v>
       </c>
       <c r="E35" t="n">
-        <v>-428</v>
+        <v>427.9999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -974,13 +974,13 @@
         <v>251</v>
       </c>
       <c r="C36" t="n">
-        <v>1.299999237060547</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>-325</v>
+        <v>325</v>
       </c>
       <c r="E36" t="n">
-        <v>-430</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37">
@@ -991,13 +991,13 @@
         <v>256</v>
       </c>
       <c r="C37" t="n">
-        <v>1.300000190734863</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>-327</v>
+        <v>327</v>
       </c>
       <c r="E37" t="n">
-        <v>-430.9999694824219</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38">
@@ -1008,13 +1008,13 @@
         <v>261</v>
       </c>
       <c r="C38" t="n">
-        <v>1.340000152587891</v>
+        <v>1.34</v>
       </c>
       <c r="D38" t="n">
-        <v>-330</v>
+        <v>330</v>
       </c>
       <c r="E38" t="n">
-        <v>-434</v>
+        <v>433.9999999999999</v>
       </c>
     </row>
     <row r="39">
@@ -1025,13 +1025,13 @@
         <v>266</v>
       </c>
       <c r="C39" t="n">
-        <v>1.200000762939453</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="D39" t="n">
-        <v>-334</v>
+        <v>333.9999999999999</v>
       </c>
       <c r="E39" t="n">
-        <v>-435</v>
+        <v>435</v>
       </c>
     </row>
     <row r="40">
@@ -1042,13 +1042,13 @@
         <v>271</v>
       </c>
       <c r="C40" t="n">
-        <v>1.199999809265137</v>
+        <v>1.200000000000001</v>
       </c>
       <c r="D40" t="n">
-        <v>-337</v>
+        <v>337</v>
       </c>
       <c r="E40" t="n">
-        <v>-437</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41">
@@ -1059,13 +1059,13 @@
         <v>276</v>
       </c>
       <c r="C41" t="n">
-        <v>1.200000762939453</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="D41" t="n">
-        <v>-342</v>
+        <v>342</v>
       </c>
       <c r="E41" t="n">
-        <v>-439</v>
+        <v>438.9999999999999</v>
       </c>
     </row>
     <row r="42">
@@ -1076,13 +1076,13 @@
         <v>283</v>
       </c>
       <c r="C42" t="n">
-        <v>1.100000381469727</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="D42" t="n">
-        <v>-348</v>
+        <v>347.9999999999999</v>
       </c>
       <c r="E42" t="n">
-        <v>-442</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43">
@@ -1093,13 +1093,13 @@
         <v>288</v>
       </c>
       <c r="C43" t="n">
-        <v>1.199999809265137</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="D43" t="n">
-        <v>-352</v>
+        <v>352</v>
       </c>
       <c r="E43" t="n">
-        <v>-444</v>
+        <v>443.9999999999999</v>
       </c>
     </row>
     <row r="44">
@@ -1110,13 +1110,13 @@
         <v>293</v>
       </c>
       <c r="C44" t="n">
-        <v>1.09999942779541</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="D44" t="n">
-        <v>-355.9999694824219</v>
+        <v>356</v>
       </c>
       <c r="E44" t="n">
-        <v>-445</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45">
@@ -1127,13 +1127,13 @@
         <v>298</v>
       </c>
       <c r="C45" t="n">
-        <v>1.199999809265137</v>
+        <v>1.2</v>
       </c>
       <c r="D45" t="n">
-        <v>-358</v>
+        <v>357.9999999999999</v>
       </c>
       <c r="E45" t="n">
-        <v>-447</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>